<commit_message>
v0.1.1 - Fix sheet names, add campaign dates, move resumen to administrador/
- Fixed sheet name mappings for updated resumen_general.xlsx
- Added /api/campaigns/dates endpoint for cut-off dates
- Campaign selector now shows fecha de corte above each card
- Moved resumen_general.xlsx to administrador/ folder
- Updated server path references
- Included dist/ build for Hostinger deployment
</commit_message>
<xml_diff>
--- a/camino_cumbre/camino_cumbre.xlsx
+++ b/camino_cumbre/camino_cumbre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/camino_cumbre/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/camino_cumbre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FD1D3B-F756-8F46-B113-1A57B23398CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4317FDCA-E879-B041-BED2-C241BC816BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Asesor</t>
   </si>
@@ -74,9 +74,6 @@
     <t>LUIS GUILLERMO OLGUIN FERNANDEZ</t>
   </si>
   <si>
-    <t>LINDA TANIA MIROSLAVA ENRIQUEZ PRECIADO</t>
-  </si>
-  <si>
     <t>HANA SOFIA LOPEZ QUIÐONEZ</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
   </si>
   <si>
     <t>ISAI ANTONIO ROJAS MARTINEZ</t>
-  </si>
-  <si>
-    <t>ROCIO IVON RUIZ GARCIA</t>
   </si>
   <si>
     <t>ANA VERONICA GONZALEZ GAYTAN</t>
@@ -1260,7 +1254,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J21"/>
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1286,28 +1280,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18">
@@ -1318,19 +1312,19 @@
         <v>110453</v>
       </c>
       <c r="C2" s="6">
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D2" s="10">
         <v>45600</v>
       </c>
       <c r="E2" s="14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="7">
         <v>5</v>
       </c>
       <c r="G2" s="15">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" s="12">
         <v>5.5</v>
@@ -1342,78 +1336,76 @@
         <v>5.5</v>
       </c>
       <c r="K2" s="11" t="str">
-        <f t="shared" ref="K2:K21" si="0">IF(G2&gt;=(E2*4),"EN META","POR DEBAJO")</f>
+        <f>IF(G2&gt;=(E2*4),"EN META","POR DEBAJO")</f>
         <v>POR DEBAJO</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5">
-        <v>108658</v>
+        <v>111056</v>
       </c>
       <c r="C3" s="6">
-        <f>C2</f>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D3" s="10">
-        <v>45497</v>
+        <v>45639</v>
       </c>
       <c r="E3" s="14">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="15">
-        <v>27.5</v>
+        <v>22.5</v>
       </c>
       <c r="H3" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I3" s="12">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="12">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="K3" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K2:K21" si="0">IF(G3&gt;=(E3*4),"EN META","POR DEBAJO")</f>
         <v>POR DEBAJO</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>110575</v>
+      </c>
+      <c r="C4" s="6">
+        <v>46053</v>
+      </c>
+      <c r="D4" s="10">
+        <v>45583</v>
+      </c>
+      <c r="E4" s="14">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
-        <v>111056</v>
-      </c>
-      <c r="C4" s="6">
-        <f t="shared" ref="C4:C21" si="1">C3</f>
-        <v>46022</v>
-      </c>
-      <c r="D4" s="10">
-        <v>45639</v>
-      </c>
-      <c r="E4" s="14">
-        <v>13</v>
-      </c>
-      <c r="F4" s="7">
-        <v>5</v>
-      </c>
       <c r="G4" s="15">
-        <v>22</v>
+        <v>21.5</v>
       </c>
       <c r="H4" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" s="12">
         <v>0.5</v>
       </c>
       <c r="J4" s="12">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1422,35 +1414,34 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5">
-        <v>110575</v>
+        <v>109998</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D5" s="10">
-        <v>45583</v>
+        <v>45596</v>
       </c>
       <c r="E5" s="14">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7">
+        <v>6</v>
+      </c>
+      <c r="G5" s="15">
+        <v>19.5</v>
+      </c>
+      <c r="H5" s="12">
         <v>5</v>
       </c>
-      <c r="G5" s="15">
-        <v>21.5</v>
-      </c>
-      <c r="H5" s="12">
-        <v>7</v>
-      </c>
       <c r="I5" s="12">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="J5" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1459,35 +1450,34 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="13" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5">
-        <v>109998</v>
+        <v>110105</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D6" s="10">
-        <v>45596</v>
+        <v>45560</v>
       </c>
       <c r="E6" s="14">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="15">
-        <v>19.5</v>
+        <v>19</v>
       </c>
       <c r="H6" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I6" s="12">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="J6" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1496,35 +1486,34 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5">
-        <v>110105</v>
+        <v>109819</v>
       </c>
       <c r="C7" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D7" s="10">
-        <v>45560</v>
+        <v>45562</v>
       </c>
       <c r="E7" s="14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="7">
         <v>6</v>
       </c>
       <c r="G7" s="15">
-        <v>19</v>
+        <v>18.5</v>
       </c>
       <c r="H7" s="12">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="I7" s="12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J7" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1533,35 +1522,34 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
-        <v>109819</v>
+        <v>114100</v>
       </c>
       <c r="C8" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D8" s="10">
-        <v>45562</v>
+        <v>45863</v>
       </c>
       <c r="E8" s="14">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F8" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G8" s="15">
-        <v>18.5</v>
+        <v>13.5</v>
       </c>
       <c r="H8" s="12">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="I8" s="12">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12">
         <v>2</v>
-      </c>
-      <c r="J8" s="12">
-        <v>0</v>
       </c>
       <c r="K8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1570,35 +1558,34 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5">
-        <v>114100</v>
+        <v>115047</v>
       </c>
       <c r="C9" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D9" s="10">
-        <v>45863</v>
+        <v>45944</v>
       </c>
       <c r="E9" s="14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
       </c>
       <c r="G9" s="15">
-        <v>13.5</v>
+        <v>13</v>
       </c>
       <c r="H9" s="12">
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
       <c r="I9" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1607,20 +1594,19 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5">
         <v>109007</v>
       </c>
       <c r="C10" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D10" s="10">
         <v>45525</v>
       </c>
       <c r="E10" s="14">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="7">
         <v>6</v>
@@ -1644,57 +1630,55 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5">
+        <v>113450</v>
+      </c>
+      <c r="C11" s="6">
+        <v>46053</v>
+      </c>
+      <c r="D11" s="10">
+        <v>45852</v>
+      </c>
+      <c r="E11" s="14">
         <v>7</v>
       </c>
-      <c r="B11" s="5">
-        <v>115047</v>
-      </c>
-      <c r="C11" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
-      </c>
-      <c r="D11" s="10">
-        <v>45944</v>
-      </c>
-      <c r="E11" s="14">
+      <c r="F11" s="7">
         <v>3</v>
       </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
       <c r="G11" s="15">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="H11" s="12">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="I11" s="12">
         <v>2</v>
       </c>
       <c r="J11" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>EN META</v>
+        <v>POR DEBAJO</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5">
         <v>111960</v>
       </c>
       <c r="C12" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D12" s="10">
         <v>45707</v>
       </c>
       <c r="E12" s="14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="7">
         <v>4</v>
@@ -1718,35 +1702,34 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5">
-        <v>113450</v>
+        <v>113076</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D13" s="10">
-        <v>45852</v>
+        <v>45806</v>
       </c>
       <c r="E13" s="14">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" s="15">
         <v>10.5</v>
       </c>
       <c r="H13" s="12">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="I13" s="12">
         <v>2</v>
       </c>
       <c r="J13" s="12">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1755,35 +1738,34 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5">
-        <v>113076</v>
+        <v>115404</v>
       </c>
       <c r="C14" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D14" s="10">
-        <v>45806</v>
+        <v>45986</v>
       </c>
       <c r="E14" s="14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>9</v>
+      </c>
+      <c r="H14" s="12">
         <v>8</v>
       </c>
-      <c r="F14" s="7">
-        <v>3</v>
-      </c>
-      <c r="G14" s="15">
-        <v>10.5</v>
-      </c>
-      <c r="H14" s="12">
-        <v>5.5</v>
-      </c>
       <c r="I14" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="12">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1792,72 +1774,70 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5">
-        <v>115404</v>
+        <v>112083</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D15" s="10">
-        <v>45986</v>
+        <v>45736</v>
       </c>
       <c r="E15" s="14">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F15" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G15" s="15">
         <v>9</v>
       </c>
       <c r="H15" s="12">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="I15" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="12">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K15" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>EN META</v>
+        <v>POR DEBAJO</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5">
-        <v>112083</v>
+        <v>114157</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D16" s="10">
-        <v>45736</v>
+        <v>45904</v>
       </c>
       <c r="E16" s="14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16" s="15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" s="12">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I16" s="12">
         <v>0</v>
       </c>
       <c r="J16" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1866,35 +1846,34 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5">
-        <v>114157</v>
+        <v>116060</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D17" s="10">
-        <v>45904</v>
+        <v>46010</v>
       </c>
       <c r="E17" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="12">
         <v>6</v>
       </c>
       <c r="I17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
         <v>0</v>
-      </c>
-      <c r="J17" s="12">
-        <v>1</v>
       </c>
       <c r="K17" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1903,20 +1882,19 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
         <v>114431</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D18" s="10">
         <v>45930</v>
       </c>
       <c r="E18" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="7">
         <v>2</v>
@@ -1940,114 +1918,65 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5">
-        <v>116060</v>
+        <v>112522</v>
       </c>
       <c r="C19" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="D19" s="10">
-        <v>46010</v>
+        <v>45776</v>
       </c>
       <c r="E19" s="14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G19" s="15">
         <v>6</v>
       </c>
       <c r="H19" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I19" s="12">
         <v>0</v>
       </c>
       <c r="J19" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K19" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>EN META</v>
+        <v>POR DEBAJO</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="5">
-        <v>112522</v>
-      </c>
-      <c r="C20" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
-      </c>
-      <c r="D20" s="10">
-        <v>45776</v>
-      </c>
-      <c r="E20" s="14">
-        <v>9</v>
-      </c>
-      <c r="F20" s="7">
-        <v>3</v>
-      </c>
-      <c r="G20" s="15">
-        <v>6</v>
-      </c>
-      <c r="H20" s="12">
-        <v>4</v>
-      </c>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-      <c r="J20" s="12">
-        <v>2</v>
-      </c>
-      <c r="K20" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>POR DEBAJO</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="5">
-        <v>114664</v>
-      </c>
-      <c r="C21" s="6">
-        <f t="shared" si="1"/>
-        <v>46022</v>
-      </c>
-      <c r="D21" s="10">
-        <v>45950</v>
-      </c>
-      <c r="E21" s="14">
-        <v>3</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="15">
-        <v>4</v>
-      </c>
-      <c r="H21" s="12">
-        <v>4</v>
-      </c>
-      <c r="I21" s="12">
-        <v>0</v>
-      </c>
-      <c r="J21" s="12">
-        <v>0</v>
-      </c>
-      <c r="K21" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>POR DEBAJO</v>
-      </c>
+      <c r="A21" s="9"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6">

</xml_diff>

<commit_message>
v0.1.5 - Updated all campaign data (Feb 18 cut-off)
- MDRT, Camino Cumbre, Convenciones, Graduación, Legión Centurión updated
- All campaigns now at Feb 18 2026 cut-off
</commit_message>
<xml_diff>
--- a/camino_cumbre/camino_cumbre.xlsx
+++ b/camino_cumbre/camino_cumbre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/camino_cumbre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4317FDCA-E879-B041-BED2-C241BC816BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6500E2E-D7F2-2342-8438-4263AC17A94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16380" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Asesor</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>CLAUDIA VALERIA HERNANDEZ MACIAS</t>
-  </si>
-  <si>
-    <t>ISAI ANTONIO ROJAS MARTINEZ</t>
   </si>
   <si>
     <t>ANA VERONICA GONZALEZ GAYTAN</t>
@@ -299,7 +296,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{0315DA01-7635-3B4E-915F-54A381A18AE8}"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="22">
     <dxf>
       <border>
         <left style="thin">
@@ -354,22 +351,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -405,54 +386,6 @@
         </top>
         <bottom style="hair">
           <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
       </border>
     </dxf>
@@ -910,23 +843,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}" name="Tabla1354" displayName="Tabla1354" ref="A1:K21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A1:K21" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K39">
-    <sortCondition descending="1" ref="G1:G39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}" name="Tabla1354" displayName="Tabla1354" ref="A1:K20" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A1:K20" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K38">
+    <sortCondition descending="1" ref="G1:G38"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F64D903D-9F21-1C46-8ECA-63392820498E}" name="Asesor" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{E38F8F07-E36B-CC43-B077-DF828B75CE31}" name="Clave" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{12677A66-E491-A149-827F-A27FD283E2FE}" name="Fecha_Corte" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{7B920709-BCF4-6E42-BB63-55BF01110007}" name="Fecha_Conexion" dataDxfId="17" dataCellStyle="Normal 2"/>
-    <tableColumn id="9" xr3:uid="{EB5FBA11-D0FE-794C-8F1D-3C3492AB053A}" name="Mes_Asesor" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="14" xr3:uid="{17B4B670-463A-8F40-996C-94559C2C6156}" name="Trimestre" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{A4DA8ED3-2571-AD46-AEE7-65DE2102D661}" name="Polizas_Totales" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="16" xr3:uid="{2103F9BE-FF32-BF42-B491-685E796B7946}" name="Mes_1_Prod" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="18" xr3:uid="{E43E2E5F-4B97-DC43-90D1-8A6AB3D848E9}" name="Mes_2_Prod" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="17" xr3:uid="{3B87E0D8-ACE3-034E-9A51-908E049FE5F8}" name="Mes_3_Prod" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{9128F4F2-9D5B-114E-AFF8-D23C1B15D538}" name="Estatus_meta" dataDxfId="10" dataCellStyle="Millares">
+    <tableColumn id="1" xr3:uid="{F64D903D-9F21-1C46-8ECA-63392820498E}" name="Asesor" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{E38F8F07-E36B-CC43-B077-DF828B75CE31}" name="Clave" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{12677A66-E491-A149-827F-A27FD283E2FE}" name="Fecha_Corte" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{7B920709-BCF4-6E42-BB63-55BF01110007}" name="Fecha_Conexion" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="9" xr3:uid="{EB5FBA11-D0FE-794C-8F1D-3C3492AB053A}" name="Mes_Asesor" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="14" xr3:uid="{17B4B670-463A-8F40-996C-94559C2C6156}" name="Trimestre" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{A4DA8ED3-2571-AD46-AEE7-65DE2102D661}" name="Polizas_Totales" dataDxfId="10" dataCellStyle="Normal 2"/>
+    <tableColumn id="16" xr3:uid="{2103F9BE-FF32-BF42-B491-685E796B7946}" name="Mes_1_Prod" dataDxfId="9" dataCellStyle="Normal 2"/>
+    <tableColumn id="18" xr3:uid="{E43E2E5F-4B97-DC43-90D1-8A6AB3D848E9}" name="Mes_2_Prod" dataDxfId="8" dataCellStyle="Normal 2"/>
+    <tableColumn id="17" xr3:uid="{3B87E0D8-ACE3-034E-9A51-908E049FE5F8}" name="Mes_3_Prod" dataDxfId="7" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{9128F4F2-9D5B-114E-AFF8-D23C1B15D538}" name="Estatus_meta" dataDxfId="6" dataCellStyle="Millares">
       <calculatedColumnFormula>IF(G2&gt;=(E2*4),"EN META","POR DEBAJO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1251,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F458E5-AEE6-2C47-8476-20D6DBF9B331}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G9"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1280,28 +1213,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18">
@@ -1312,19 +1245,19 @@
         <v>110453</v>
       </c>
       <c r="C2" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D2" s="10">
         <v>45600</v>
       </c>
       <c r="E2" s="14">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="15">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H2" s="12">
         <v>5.5</v>
@@ -1348,19 +1281,19 @@
         <v>111056</v>
       </c>
       <c r="C3" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D3" s="10">
         <v>45639</v>
       </c>
       <c r="E3" s="14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="7">
         <v>5</v>
       </c>
       <c r="G3" s="15">
-        <v>22.5</v>
+        <v>23</v>
       </c>
       <c r="H3" s="12">
         <v>8</v>
@@ -1372,7 +1305,7 @@
         <v>3.5</v>
       </c>
       <c r="K3" s="8" t="str">
-        <f t="shared" ref="K2:K21" si="0">IF(G3&gt;=(E3*4),"EN META","POR DEBAJO")</f>
+        <f t="shared" ref="K3:K18" si="0">IF(G3&gt;=(E3*4),"EN META","POR DEBAJO")</f>
         <v>POR DEBAJO</v>
       </c>
     </row>
@@ -1384,13 +1317,13 @@
         <v>110575</v>
       </c>
       <c r="C4" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D4" s="10">
         <v>45583</v>
       </c>
       <c r="E4" s="14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="7">
         <v>6</v>
@@ -1414,19 +1347,19 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
-        <v>109998</v>
+        <v>110105</v>
       </c>
       <c r="C5" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D5" s="10">
-        <v>45596</v>
+        <v>45560</v>
       </c>
       <c r="E5" s="14">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5" s="7">
         <v>6</v>
@@ -1435,13 +1368,13 @@
         <v>19.5</v>
       </c>
       <c r="H5" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="12">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="J5" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1450,16 +1383,16 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="13" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5">
-        <v>110105</v>
+        <v>109998</v>
       </c>
       <c r="C6" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D6" s="10">
-        <v>45560</v>
+        <v>45596</v>
       </c>
       <c r="E6" s="14">
         <v>17</v>
@@ -1468,16 +1401,16 @@
         <v>6</v>
       </c>
       <c r="G6" s="15">
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="H6" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J6" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1492,13 +1425,13 @@
         <v>109819</v>
       </c>
       <c r="C7" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D7" s="10">
         <v>45562</v>
       </c>
       <c r="E7" s="14">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7">
         <v>6</v>
@@ -1522,34 +1455,34 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>114100</v>
+        <v>115047</v>
       </c>
       <c r="C8" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D8" s="10">
-        <v>45863</v>
+        <v>45944</v>
       </c>
       <c r="E8" s="14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="15">
         <v>13.5</v>
       </c>
       <c r="H8" s="12">
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
       <c r="I8" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1558,34 +1491,34 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>115047</v>
+        <v>114100</v>
       </c>
       <c r="C9" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D9" s="10">
-        <v>45944</v>
+        <v>45863</v>
       </c>
       <c r="E9" s="14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F9" s="7">
+        <v>3</v>
+      </c>
+      <c r="G9" s="15">
+        <v>13.5</v>
+      </c>
+      <c r="H9" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
         <v>2</v>
-      </c>
-      <c r="G9" s="15">
-        <v>13</v>
-      </c>
-      <c r="H9" s="12">
-        <v>8.5</v>
-      </c>
-      <c r="I9" s="12">
-        <v>2</v>
-      </c>
-      <c r="J9" s="12">
-        <v>1.5</v>
       </c>
       <c r="K9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1594,34 +1527,34 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5">
-        <v>109007</v>
+        <v>113450</v>
       </c>
       <c r="C10" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D10" s="10">
-        <v>45525</v>
+        <v>45852</v>
       </c>
       <c r="E10" s="14">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F10" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G10" s="15">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="H10" s="12">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="I10" s="12">
         <v>2</v>
       </c>
       <c r="J10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1630,34 +1563,34 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5">
-        <v>113450</v>
+        <v>111960</v>
       </c>
       <c r="C11" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D11" s="10">
-        <v>45852</v>
+        <v>45707</v>
       </c>
       <c r="E11" s="14">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F11" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G11" s="15">
         <v>11.5</v>
       </c>
       <c r="H11" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I11" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1666,34 +1599,34 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5">
-        <v>111960</v>
+        <v>113076</v>
       </c>
       <c r="C12" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D12" s="10">
-        <v>45707</v>
+        <v>45806</v>
       </c>
       <c r="E12" s="14">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="7">
         <v>4</v>
       </c>
       <c r="G12" s="15">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="H12" s="12">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="I12" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" s="12">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1702,34 +1635,34 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5">
-        <v>113076</v>
+        <v>115404</v>
       </c>
       <c r="C13" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D13" s="10">
-        <v>45806</v>
+        <v>45986</v>
       </c>
       <c r="E13" s="14">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F13" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" s="15">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="H13" s="12">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="I13" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="12">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1738,34 +1671,34 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B14" s="5">
-        <v>115404</v>
+        <v>112083</v>
       </c>
       <c r="C14" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D14" s="10">
-        <v>45986</v>
+        <v>45736</v>
       </c>
       <c r="E14" s="14">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F14" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G14" s="15">
         <v>9</v>
       </c>
       <c r="H14" s="12">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="I14" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="12">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1774,31 +1707,31 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5">
-        <v>112083</v>
+        <v>116060</v>
       </c>
       <c r="C15" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D15" s="10">
-        <v>45736</v>
+        <v>46010</v>
       </c>
       <c r="E15" s="14">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F15" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G15" s="15">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="H15" s="12">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="12">
         <v>1.5</v>
@@ -1816,13 +1749,13 @@
         <v>114157</v>
       </c>
       <c r="C16" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D16" s="10">
         <v>45904</v>
       </c>
       <c r="E16" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F16" s="7">
         <v>2</v>
@@ -1846,31 +1779,31 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5">
-        <v>116060</v>
+        <v>114431</v>
       </c>
       <c r="C17" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D17" s="10">
-        <v>46010</v>
+        <v>45930</v>
       </c>
       <c r="E17" s="14">
+        <v>6</v>
+      </c>
+      <c r="F17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
       <c r="G17" s="15">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="H17" s="12">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="I17" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="12">
         <v>0</v>
@@ -1882,34 +1815,34 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B18" s="5">
-        <v>114431</v>
+        <v>112522</v>
       </c>
       <c r="C18" s="6">
-        <v>46053</v>
+        <v>46071</v>
       </c>
       <c r="D18" s="10">
-        <v>45930</v>
+        <v>45776</v>
       </c>
       <c r="E18" s="14">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F18" s="7">
+        <v>4</v>
+      </c>
+      <c r="G18" s="15">
+        <v>6</v>
+      </c>
+      <c r="H18" s="12">
+        <v>4</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
         <v>2</v>
-      </c>
-      <c r="G18" s="15">
-        <v>6.5</v>
-      </c>
-      <c r="H18" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="I18" s="12">
-        <v>2</v>
-      </c>
-      <c r="J18" s="12">
-        <v>0</v>
       </c>
       <c r="K18" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1917,43 +1850,20 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="5">
-        <v>112522</v>
-      </c>
-      <c r="C19" s="6">
-        <v>46053</v>
-      </c>
-      <c r="D19" s="10">
-        <v>45776</v>
-      </c>
-      <c r="E19" s="14">
-        <v>10</v>
-      </c>
-      <c r="F19" s="7">
-        <v>4</v>
-      </c>
-      <c r="G19" s="15">
-        <v>6</v>
-      </c>
-      <c r="H19" s="12">
-        <v>4</v>
-      </c>
-      <c r="I19" s="12">
-        <v>0</v>
-      </c>
-      <c r="J19" s="12">
-        <v>2</v>
-      </c>
-      <c r="K19" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>POR DEBAJO</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="4"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="10"/>
@@ -1965,66 +1875,33 @@
       <c r="J20" s="12"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="9"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="8"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="A6 F2:F20 C2:C20">
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C21 F2:F21">
-    <cfRule type="expression" dxfId="8" priority="23" stopIfTrue="1">
-      <formula>#REF!&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D21">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:E20 G2:J20">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>$B2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
-      <formula>$B2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="H2:H20">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$Z2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:J21">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
-      <formula>$B2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$AA2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="expression" priority="3" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$AB2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K21">
+  <conditionalFormatting sqref="K3:K20">
     <cfRule type="expression" dxfId="1" priority="21" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>

</xml_diff>